<commit_message>
Basic load combinations generator
</commit_message>
<xml_diff>
--- a/m100_Tools_And_Helpers/11 Loadcases.xlsx
+++ b/m100_Tools_And_Helpers/11 Loadcases.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\m100_Tools_And_Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0027CD0-63D1-46F3-8C5D-7D4FF85B5DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8320B6FE-D7D5-499D-8C5F-A8D632CB8FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9240" yWindow="1872" windowWidth="13488" windowHeight="10332" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loadcases" sheetId="1" r:id="rId1"/>
     <sheet name="Envelopes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Self Weight</t>
   </si>
@@ -76,9 +87,6 @@
     <t>FindSimilar</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Traffic 1</t>
   </si>
   <si>
@@ -134,6 +142,33 @@
   </si>
   <si>
     <t>Gravity = Automatically apply gravity to the loadcase</t>
+  </si>
+  <si>
+    <t>Settlement Envelope</t>
+  </si>
+  <si>
+    <t>Wind Envelope</t>
+  </si>
+  <si>
+    <t>TLO Traffic Envelope</t>
+  </si>
+  <si>
+    <t>Thermal Envelope</t>
+  </si>
+  <si>
+    <t>Rail Load Characteristic</t>
+  </si>
+  <si>
+    <t>Track 1</t>
+  </si>
+  <si>
+    <t>Rail Track Up</t>
+  </si>
+  <si>
+    <t>Rail Track Down</t>
+  </si>
+  <si>
+    <t>Track 2</t>
   </si>
 </sst>
 </file>
@@ -479,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,7 +535,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -514,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -522,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -530,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -541,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -583,16 +618,39 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -600,17 +658,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803832CE-E52E-47CE-865F-4A6C7DB9A262}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
     <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -626,7 +684,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -635,12 +693,12 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -649,12 +707,12 @@
         <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -663,87 +721,109 @@
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Accidental and Seismic combinations
</commit_message>
<xml_diff>
--- a/m100_Tools_And_Helpers/11 Loadcases.xlsx
+++ b/m100_Tools_And_Helpers/11 Loadcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\m100_Tools_And_Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEF62B2-8E0A-437F-9309-CFDC03549B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428C9DD3-1805-49D4-BF34-E5A9EC6EFC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loadcases" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Self Weight</t>
   </si>
@@ -183,10 +183,37 @@
     <t>Folder = Folder for grouping envelopes in tree view</t>
   </si>
   <si>
-    <t>Variable Actions</t>
-  </si>
-  <si>
-    <t>Permanent Actions</t>
+    <t>Explosion</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Explosion Envelope</t>
+  </si>
+  <si>
+    <t>Impact Envelope</t>
+  </si>
+  <si>
+    <t>Seismic</t>
+  </si>
+  <si>
+    <t>Seismic Analysis</t>
+  </si>
+  <si>
+    <t>Seismic Envelope</t>
+  </si>
+  <si>
+    <t>00 Permanent Actions</t>
+  </si>
+  <si>
+    <t>01 Variable Actions</t>
+  </si>
+  <si>
+    <t>02 Accidental Actions</t>
+  </si>
+  <si>
+    <t>03 Seismic Actions</t>
   </si>
 </sst>
 </file>
@@ -532,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,6 +694,33 @@
         <v>39</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -676,10 +730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803832CE-E52E-47CE-865F-4A6C7DB9A262}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>26</v>
@@ -732,7 +786,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>27</v>
@@ -749,7 +803,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>28</v>
@@ -763,7 +817,7 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>47</v>
@@ -777,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -788,7 +842,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -799,7 +853,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -810,7 +864,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -821,7 +875,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -832,7 +886,7 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -843,7 +897,7 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -854,7 +908,7 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -865,7 +919,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -879,7 +933,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -893,7 +947,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -907,7 +961,49 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>